<commit_message>
modularizaion al wordix.php,falta funcion (1,9,11)
</commit_message>
<xml_diff>
--- a/estructurasDatosWordix.xlsx
+++ b/estructurasDatosWordix.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6EFA76C-4C6E-4342-95A9-2FB779FEDEF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EstructuraDatos" sheetId="1" r:id="rId1"/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="66">
   <si>
     <t>$coleccionPalabras=</t>
   </si>
@@ -46,15 +47,6 @@
     <t>Información de la estructura:</t>
   </si>
   <si>
-    <t>//indices</t>
-  </si>
-  <si>
-    <t>//valores</t>
-  </si>
-  <si>
-    <t>**** COMPLETAR ****</t>
-  </si>
-  <si>
     <t>Ejemplo de cómo representar las estructuras de datos según lo visto en teoría:</t>
   </si>
   <si>
@@ -62,13 +54,172 @@
   </si>
   <si>
     <t>¿Para qué se utiliza?: guarda las palabras que se pueden elegidas para jugar wordix</t>
+  </si>
+  <si>
+    <t>HUEVO</t>
+  </si>
+  <si>
+    <t>TINTO</t>
+  </si>
+  <si>
+    <t>VERDE</t>
+  </si>
+  <si>
+    <t>MELON</t>
+  </si>
+  <si>
+    <t>YUYOS</t>
+  </si>
+  <si>
+    <t>PIANO</t>
+  </si>
+  <si>
+    <t>PISOS</t>
+  </si>
+  <si>
+    <t>CEBRA</t>
+  </si>
+  <si>
+    <t>MANGO</t>
+  </si>
+  <si>
+    <t>LINCE</t>
+  </si>
+  <si>
+    <t>FLAMA</t>
+  </si>
+  <si>
+    <t>GRANO</t>
+  </si>
+  <si>
+    <t>"intentos"</t>
+  </si>
+  <si>
+    <t>"jugador"</t>
+  </si>
+  <si>
+    <t>"palabraWordix"</t>
+  </si>
+  <si>
+    <t>queso</t>
+  </si>
+  <si>
+    <t>majo</t>
+  </si>
+  <si>
+    <t>"puntaje"</t>
+  </si>
+  <si>
+    <t>casas</t>
+  </si>
+  <si>
+    <t>rudolf</t>
+  </si>
+  <si>
+    <t>pink2000</t>
+  </si>
+  <si>
+    <t>mujer</t>
+  </si>
+  <si>
+    <t>huevo</t>
+  </si>
+  <si>
+    <t>tinto</t>
+  </si>
+  <si>
+    <t>verde</t>
+  </si>
+  <si>
+    <t>melon</t>
+  </si>
+  <si>
+    <t>yuyos</t>
+  </si>
+  <si>
+    <t>pisos</t>
+  </si>
+  <si>
+    <t>cebra</t>
+  </si>
+  <si>
+    <t>migue</t>
+  </si>
+  <si>
+    <t>migue1</t>
+  </si>
+  <si>
+    <t>clara</t>
+  </si>
+  <si>
+    <t>clara2</t>
+  </si>
+  <si>
+    <t>gordo1</t>
+  </si>
+  <si>
+    <t>gordo2</t>
+  </si>
+  <si>
+    <t>diego</t>
+  </si>
+  <si>
+    <t>diego2</t>
+  </si>
+  <si>
+    <t>informacion de la estructura:</t>
+  </si>
+  <si>
+    <t>Tipo: multidimensional(indexado por asociativo)</t>
+  </si>
+  <si>
+    <t>Tipos de datos: Almacena valores String y enteros</t>
+  </si>
+  <si>
+    <t>almacena informacion de las partidas que se jugaron</t>
+  </si>
+  <si>
+    <t>resumenJugador=</t>
+  </si>
+  <si>
+    <t>colecciónPartidas=</t>
+  </si>
+  <si>
+    <t>"partidas"</t>
+  </si>
+  <si>
+    <t>"victorias"</t>
+  </si>
+  <si>
+    <t>"intento1 "</t>
+  </si>
+  <si>
+    <t>"intento2"</t>
+  </si>
+  <si>
+    <t>"intento3"</t>
+  </si>
+  <si>
+    <t>"intento4"</t>
+  </si>
+  <si>
+    <t>"intento5"</t>
+  </si>
+  <si>
+    <t>"intento6"</t>
+  </si>
+  <si>
+    <t>Tipo: asociativo</t>
+  </si>
+  <si>
+    <t>guarda el resumen de un jugador</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,16 +244,37 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="10"/>
-      <color rgb="FF00B050"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -116,7 +288,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -139,50 +311,52 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -220,7 +394,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -254,6 +428,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -288,9 +463,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -463,107 +639,518 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:V30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.88671875" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>0</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>1</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>2</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>3</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <v>4</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="1">
         <v>5</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="6">
+        <v>6</v>
+      </c>
+      <c r="I3" s="1">
+        <v>7</v>
+      </c>
+      <c r="J3" s="1">
+        <v>8</v>
+      </c>
+      <c r="K3" s="1">
+        <v>9</v>
+      </c>
+      <c r="L3" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="B4" s="1" t="s">
+      <c r="M3" s="1">
+        <v>11</v>
+      </c>
+      <c r="N3" s="1">
+        <v>12</v>
+      </c>
+      <c r="O3" s="1">
+        <v>13</v>
+      </c>
+      <c r="P3" s="1">
+        <v>14</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>15</v>
+      </c>
+      <c r="R3" s="1">
+        <v>16</v>
+      </c>
+      <c r="S3" s="1">
+        <v>17</v>
+      </c>
+      <c r="T3" s="1">
+        <v>18</v>
+      </c>
+      <c r="U3" s="1">
+        <v>19</v>
+      </c>
+      <c r="V3" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
-      <c r="B6" s="3" t="s">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="7">
+        <v>0</v>
+      </c>
+      <c r="C13" s="7">
+        <v>1</v>
+      </c>
+      <c r="D13" s="7">
+        <v>2</v>
+      </c>
+      <c r="E13" s="7">
+        <v>3</v>
+      </c>
+      <c r="F13" s="9">
+        <v>4</v>
+      </c>
+      <c r="G13" s="7">
+        <v>5</v>
+      </c>
+      <c r="H13" s="7">
+        <v>6</v>
+      </c>
+      <c r="I13" s="7">
+        <v>7</v>
+      </c>
+      <c r="J13" s="7">
+        <v>8</v>
+      </c>
+      <c r="K13" s="7">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="B8" t="s">
+      <c r="L13" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="L14" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="L15" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="7">
+        <v>0</v>
+      </c>
+      <c r="C16" s="7">
+        <v>3</v>
+      </c>
+      <c r="D16" s="7">
+        <v>6</v>
+      </c>
+      <c r="E16" s="7">
+        <v>1</v>
+      </c>
+      <c r="F16" s="7">
+        <v>2</v>
+      </c>
+      <c r="G16" s="7">
+        <v>3</v>
+      </c>
+      <c r="H16" s="7">
+        <v>4</v>
+      </c>
+      <c r="I16" s="7">
+        <v>5</v>
+      </c>
+      <c r="J16" s="7">
+        <v>6</v>
+      </c>
+      <c r="K16" s="7">
+        <v>2</v>
+      </c>
+      <c r="L16" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="7">
+        <v>0</v>
+      </c>
+      <c r="C17" s="7">
+        <v>14</v>
+      </c>
+      <c r="D17" s="7">
+        <v>10</v>
+      </c>
+      <c r="E17" s="7">
+        <v>15</v>
+      </c>
+      <c r="F17" s="7">
+        <v>13</v>
+      </c>
+      <c r="G17" s="7">
+        <v>15</v>
+      </c>
+      <c r="H17" s="7">
+        <v>13</v>
+      </c>
+      <c r="I17" s="7">
+        <v>11</v>
+      </c>
+      <c r="J17" s="7">
+        <v>12</v>
+      </c>
+      <c r="K17" s="7">
+        <v>16</v>
+      </c>
+      <c r="L17" s="7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B19" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B20" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B21" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B22" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="J24" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="K24" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B25" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="7">
+        <v>2</v>
+      </c>
+      <c r="D25" s="7">
+        <v>16</v>
+      </c>
+      <c r="E25" s="7">
+        <v>1</v>
+      </c>
+      <c r="F25" s="7">
+        <v>0</v>
+      </c>
+      <c r="G25" s="7">
+        <v>1</v>
+      </c>
+      <c r="H25" s="7">
+        <v>0</v>
+      </c>
+      <c r="I25" s="7">
+        <v>0</v>
+      </c>
+      <c r="J25" s="7">
+        <v>0</v>
+      </c>
+      <c r="K25" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B27" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B28" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B29" s="7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B30" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Completé un poco la biblioteca wordix
</commit_message>
<xml_diff>
--- a/estructurasDatosWordix.xlsx
+++ b/estructurasDatosWordix.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D96BF53A-B928-4760-BE06-E6B190A3282C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EstructuraDatos" sheetId="1" r:id="rId1"/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="66">
   <si>
     <t>$coleccionPalabras=</t>
   </si>
@@ -46,15 +47,6 @@
     <t>Información de la estructura:</t>
   </si>
   <si>
-    <t>//indices</t>
-  </si>
-  <si>
-    <t>//valores</t>
-  </si>
-  <si>
-    <t>**** COMPLETAR ****</t>
-  </si>
-  <si>
     <t>Ejemplo de cómo representar las estructuras de datos según lo visto en teoría:</t>
   </si>
   <si>
@@ -62,13 +54,172 @@
   </si>
   <si>
     <t>¿Para qué se utiliza?: guarda las palabras que se pueden elegidas para jugar wordix</t>
+  </si>
+  <si>
+    <t>HUEVO</t>
+  </si>
+  <si>
+    <t>TINTO</t>
+  </si>
+  <si>
+    <t>VERDE</t>
+  </si>
+  <si>
+    <t>MELON</t>
+  </si>
+  <si>
+    <t>YUYOS</t>
+  </si>
+  <si>
+    <t>PIANO</t>
+  </si>
+  <si>
+    <t>PISOS</t>
+  </si>
+  <si>
+    <t>CEBRA</t>
+  </si>
+  <si>
+    <t>MANGO</t>
+  </si>
+  <si>
+    <t>LINCE</t>
+  </si>
+  <si>
+    <t>FLAMA</t>
+  </si>
+  <si>
+    <t>GRANO</t>
+  </si>
+  <si>
+    <t>"intentos"</t>
+  </si>
+  <si>
+    <t>"jugador"</t>
+  </si>
+  <si>
+    <t>"palabraWordix"</t>
+  </si>
+  <si>
+    <t>queso</t>
+  </si>
+  <si>
+    <t>majo</t>
+  </si>
+  <si>
+    <t>"puntaje"</t>
+  </si>
+  <si>
+    <t>casas</t>
+  </si>
+  <si>
+    <t>rudolf</t>
+  </si>
+  <si>
+    <t>pink2000</t>
+  </si>
+  <si>
+    <t>mujer</t>
+  </si>
+  <si>
+    <t>huevo</t>
+  </si>
+  <si>
+    <t>tinto</t>
+  </si>
+  <si>
+    <t>verde</t>
+  </si>
+  <si>
+    <t>melon</t>
+  </si>
+  <si>
+    <t>yuyos</t>
+  </si>
+  <si>
+    <t>pisos</t>
+  </si>
+  <si>
+    <t>cebra</t>
+  </si>
+  <si>
+    <t>migue</t>
+  </si>
+  <si>
+    <t>migue1</t>
+  </si>
+  <si>
+    <t>clara</t>
+  </si>
+  <si>
+    <t>clara2</t>
+  </si>
+  <si>
+    <t>gordo1</t>
+  </si>
+  <si>
+    <t>gordo2</t>
+  </si>
+  <si>
+    <t>diego</t>
+  </si>
+  <si>
+    <t>diego2</t>
+  </si>
+  <si>
+    <t>informacion de la estructura:</t>
+  </si>
+  <si>
+    <t>Tipo: multidimensional(indexado por asociativo)</t>
+  </si>
+  <si>
+    <t>Tipos de datos: Almacena valores String y enteros</t>
+  </si>
+  <si>
+    <t>almacena informacion de las partidas que se jugaron</t>
+  </si>
+  <si>
+    <t>resumenJugador=</t>
+  </si>
+  <si>
+    <t>colecciónPartidas=</t>
+  </si>
+  <si>
+    <t>"partidas"</t>
+  </si>
+  <si>
+    <t>"victorias"</t>
+  </si>
+  <si>
+    <t>"intento1 "</t>
+  </si>
+  <si>
+    <t>"intento2"</t>
+  </si>
+  <si>
+    <t>"intento3"</t>
+  </si>
+  <si>
+    <t>"intento4"</t>
+  </si>
+  <si>
+    <t>"intento5"</t>
+  </si>
+  <si>
+    <t>"intento6"</t>
+  </si>
+  <si>
+    <t>Tipo: asociativo</t>
+  </si>
+  <si>
+    <t>guarda el resumen de un jugador</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,16 +244,37 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="10"/>
-      <color rgb="FF00B050"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -116,7 +288,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -139,50 +311,54 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -220,7 +396,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -254,6 +430,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -288,9 +465,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -463,107 +641,518 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:V30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.88671875" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>0</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>1</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>2</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>3</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <v>4</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="1">
         <v>5</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="7">
+        <v>6</v>
+      </c>
+      <c r="I3" s="1">
+        <v>7</v>
+      </c>
+      <c r="J3" s="1">
+        <v>8</v>
+      </c>
+      <c r="K3" s="1">
+        <v>9</v>
+      </c>
+      <c r="L3" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="B4" s="1" t="s">
+      <c r="M3" s="1">
+        <v>11</v>
+      </c>
+      <c r="N3" s="1">
+        <v>12</v>
+      </c>
+      <c r="O3" s="1">
+        <v>13</v>
+      </c>
+      <c r="P3" s="1">
+        <v>14</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>15</v>
+      </c>
+      <c r="R3" s="1">
+        <v>16</v>
+      </c>
+      <c r="S3" s="1">
+        <v>17</v>
+      </c>
+      <c r="T3" s="1">
+        <v>18</v>
+      </c>
+      <c r="U3" s="1">
+        <v>19</v>
+      </c>
+      <c r="V3" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B6" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B8" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B9" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
-      <c r="B6" s="3" t="s">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="8">
+        <v>0</v>
+      </c>
+      <c r="C13" s="8">
+        <v>1</v>
+      </c>
+      <c r="D13" s="8">
+        <v>2</v>
+      </c>
+      <c r="E13" s="8">
+        <v>3</v>
+      </c>
+      <c r="F13" s="8">
+        <v>4</v>
+      </c>
+      <c r="G13" s="8">
+        <v>5</v>
+      </c>
+      <c r="H13" s="8">
+        <v>6</v>
+      </c>
+      <c r="I13" s="8">
+        <v>7</v>
+      </c>
+      <c r="J13" s="8">
+        <v>8</v>
+      </c>
+      <c r="K13" s="8">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="B8" t="s">
+      <c r="L13" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="K14" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="L14" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="K15" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="L15" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="8">
+        <v>0</v>
+      </c>
+      <c r="C16" s="8">
+        <v>3</v>
+      </c>
+      <c r="D16" s="8">
+        <v>6</v>
+      </c>
+      <c r="E16" s="8">
+        <v>1</v>
+      </c>
+      <c r="F16" s="8">
+        <v>2</v>
+      </c>
+      <c r="G16" s="8">
+        <v>3</v>
+      </c>
+      <c r="H16" s="8">
+        <v>4</v>
+      </c>
+      <c r="I16" s="8">
+        <v>5</v>
+      </c>
+      <c r="J16" s="8">
+        <v>6</v>
+      </c>
+      <c r="K16" s="8">
+        <v>2</v>
+      </c>
+      <c r="L16" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="8">
+        <v>0</v>
+      </c>
+      <c r="C17" s="8">
+        <v>14</v>
+      </c>
+      <c r="D17" s="8">
+        <v>10</v>
+      </c>
+      <c r="E17" s="8">
+        <v>15</v>
+      </c>
+      <c r="F17" s="8">
+        <v>13</v>
+      </c>
+      <c r="G17" s="8">
+        <v>15</v>
+      </c>
+      <c r="H17" s="8">
+        <v>13</v>
+      </c>
+      <c r="I17" s="8">
+        <v>11</v>
+      </c>
+      <c r="J17" s="8">
+        <v>12</v>
+      </c>
+      <c r="K17" s="8">
+        <v>16</v>
+      </c>
+      <c r="L17" s="8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B19" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B20" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B21" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B22" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="H24" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="I24" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="J24" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="K24" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B25" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="8">
+        <v>2</v>
+      </c>
+      <c r="D25" s="8">
+        <v>16</v>
+      </c>
+      <c r="E25" s="8">
+        <v>1</v>
+      </c>
+      <c r="F25" s="8">
+        <v>0</v>
+      </c>
+      <c r="G25" s="8">
+        <v>1</v>
+      </c>
+      <c r="H25" s="8">
+        <v>0</v>
+      </c>
+      <c r="I25" s="8">
+        <v>0</v>
+      </c>
+      <c r="J25" s="8">
+        <v>0</v>
+      </c>
+      <c r="K25" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B27" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B28" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B29" s="8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B30" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>